<commit_message>
lock in current version
</commit_message>
<xml_diff>
--- a/sequences/01_cues.xlsx
+++ b/sequences/01_cues.xlsx
@@ -28,250 +28,250 @@
     <t>wenden</t>
   </si>
   <si>
+    <t>heben</t>
+  </si>
+  <si>
+    <t>drücken</t>
+  </si>
+  <si>
+    <t>rufen</t>
+  </si>
+  <si>
+    <t>buchen</t>
+  </si>
+  <si>
+    <t>sehen</t>
+  </si>
+  <si>
+    <t>enden</t>
+  </si>
+  <si>
+    <t>beißen</t>
+  </si>
+  <si>
+    <t>küssen</t>
+  </si>
+  <si>
+    <t>opfern</t>
+  </si>
+  <si>
+    <t>lehnen</t>
+  </si>
+  <si>
+    <t>tragen</t>
+  </si>
+  <si>
+    <t>schalten</t>
+  </si>
+  <si>
+    <t>pflegen</t>
+  </si>
+  <si>
+    <t>leuchten</t>
+  </si>
+  <si>
+    <t>klagen</t>
+  </si>
+  <si>
+    <t>hoffen</t>
+  </si>
+  <si>
+    <t>münzen</t>
+  </si>
+  <si>
+    <t>sparen</t>
+  </si>
+  <si>
+    <t>wandern</t>
+  </si>
+  <si>
+    <t>helfen</t>
+  </si>
+  <si>
+    <t>hören</t>
+  </si>
+  <si>
+    <t>spielen</t>
+  </si>
+  <si>
+    <t>bieten</t>
+  </si>
+  <si>
+    <t>drohen</t>
+  </si>
+  <si>
+    <t>geben</t>
+  </si>
+  <si>
+    <t>tanzen</t>
+  </si>
+  <si>
+    <t>orten</t>
+  </si>
+  <si>
+    <t>schützen</t>
+  </si>
+  <si>
     <t>treten</t>
   </si>
   <si>
+    <t>weigern</t>
+  </si>
+  <si>
+    <t>planen</t>
+  </si>
+  <si>
+    <t>binden</t>
+  </si>
+  <si>
+    <t>ächzen</t>
+  </si>
+  <si>
+    <t>kehren</t>
+  </si>
+  <si>
+    <t>dürfen</t>
+  </si>
+  <si>
+    <t>kosten</t>
+  </si>
+  <si>
+    <t>schweben</t>
+  </si>
+  <si>
+    <t>wundern</t>
+  </si>
+  <si>
+    <t>dauern</t>
+  </si>
+  <si>
+    <t>handeln</t>
+  </si>
+  <si>
+    <t>seufzen</t>
+  </si>
+  <si>
+    <t>stören</t>
+  </si>
+  <si>
+    <t>knien</t>
+  </si>
+  <si>
+    <t>biegen</t>
+  </si>
+  <si>
+    <t>bremsen</t>
+  </si>
+  <si>
+    <t>erben</t>
+  </si>
+  <si>
     <t>schulden</t>
   </si>
   <si>
-    <t>rufen</t>
-  </si>
-  <si>
-    <t>runden</t>
-  </si>
-  <si>
-    <t>holen</t>
-  </si>
-  <si>
-    <t>enden</t>
-  </si>
-  <si>
-    <t>reizen</t>
-  </si>
-  <si>
-    <t>tanzen</t>
-  </si>
-  <si>
-    <t>opfern</t>
-  </si>
-  <si>
-    <t>steuern</t>
-  </si>
-  <si>
-    <t>fügen</t>
-  </si>
-  <si>
-    <t>schalten</t>
-  </si>
-  <si>
-    <t>klingen</t>
-  </si>
-  <si>
-    <t>schwimmen</t>
-  </si>
-  <si>
-    <t>klagen</t>
-  </si>
-  <si>
-    <t>bieten</t>
-  </si>
-  <si>
-    <t>schicken</t>
-  </si>
-  <si>
-    <t>sparen</t>
-  </si>
-  <si>
-    <t>helfen</t>
-  </si>
-  <si>
-    <t>altern</t>
-  </si>
-  <si>
-    <t>hören</t>
-  </si>
-  <si>
-    <t>knien</t>
-  </si>
-  <si>
-    <t>segnen</t>
-  </si>
-  <si>
-    <t>drohen</t>
-  </si>
-  <si>
-    <t>husten</t>
-  </si>
-  <si>
-    <t>sehen</t>
-  </si>
-  <si>
-    <t>orten</t>
-  </si>
-  <si>
-    <t>dürfen</t>
-  </si>
-  <si>
-    <t>geben</t>
-  </si>
-  <si>
-    <t>weigern</t>
-  </si>
-  <si>
-    <t>spielen</t>
-  </si>
-  <si>
-    <t>binden</t>
-  </si>
-  <si>
-    <t>ächzen</t>
-  </si>
-  <si>
-    <t>werden</t>
-  </si>
-  <si>
-    <t>pflegen</t>
-  </si>
-  <si>
-    <t>kosten</t>
-  </si>
-  <si>
-    <t>heben</t>
-  </si>
-  <si>
-    <t>bilden</t>
-  </si>
-  <si>
-    <t>dauern</t>
-  </si>
-  <si>
-    <t>bauen</t>
-  </si>
-  <si>
-    <t>schneiden</t>
-  </si>
-  <si>
-    <t>stören</t>
-  </si>
-  <si>
-    <t>parken</t>
-  </si>
-  <si>
-    <t>schultern</t>
-  </si>
-  <si>
-    <t>bremsen</t>
-  </si>
-  <si>
-    <t>rasen</t>
-  </si>
-  <si>
-    <t>tragen</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
+    <t>face/face022.jpg</t>
+  </si>
+  <si>
+    <t>face/face024.jpg</t>
+  </si>
+  <si>
+    <t>house/house004.jpg</t>
+  </si>
+  <si>
+    <t>house/house009.jpg</t>
+  </si>
+  <si>
+    <t>face/face005.jpg</t>
+  </si>
+  <si>
+    <t>house/house014.jpg</t>
+  </si>
+  <si>
+    <t>house/house005.jpg</t>
+  </si>
+  <si>
+    <t>face/face002.jpg</t>
+  </si>
+  <si>
+    <t>house/house020.jpg</t>
+  </si>
+  <si>
     <t>house/house001.jpg</t>
   </si>
   <si>
-    <t>house/house010.jpg</t>
+    <t>face/face028.jpg</t>
+  </si>
+  <si>
+    <t>face/face026.jpg</t>
+  </si>
+  <si>
+    <t>house/house025.jpg</t>
+  </si>
+  <si>
+    <t>house/house019.jpg</t>
+  </si>
+  <si>
+    <t>face/face031.jpg</t>
+  </si>
+  <si>
+    <t>face/face011.jpg</t>
+  </si>
+  <si>
+    <t>face/face003.jpg</t>
+  </si>
+  <si>
+    <t>house/house008.jpg</t>
+  </si>
+  <si>
+    <t>face/face018.jpg</t>
+  </si>
+  <si>
+    <t>house/house011.jpg</t>
+  </si>
+  <si>
+    <t>house/house012.jpg</t>
+  </si>
+  <si>
+    <t>house/house018.jpg</t>
+  </si>
+  <si>
+    <t>face/face001.jpg</t>
+  </si>
+  <si>
+    <t>face/face008.jpg</t>
+  </si>
+  <si>
+    <t>house/house000.jpg</t>
+  </si>
+  <si>
+    <t>house/house028.jpg</t>
+  </si>
+  <si>
+    <t>face/face014.jpg</t>
+  </si>
+  <si>
+    <t>face/face009.jpg</t>
   </si>
   <si>
     <t>face/face007.jpg</t>
   </si>
   <si>
-    <t>house/house026.jpg</t>
-  </si>
-  <si>
-    <t>house/house013.jpg</t>
-  </si>
-  <si>
-    <t>house/house006.jpg</t>
-  </si>
-  <si>
-    <t>face/face017.jpg</t>
-  </si>
-  <si>
-    <t>face/face014.jpg</t>
-  </si>
-  <si>
-    <t>face/face021.jpg</t>
-  </si>
-  <si>
-    <t>face/face018.jpg</t>
-  </si>
-  <si>
-    <t>face/face016.jpg</t>
-  </si>
-  <si>
-    <t>house/house023.jpg</t>
-  </si>
-  <si>
-    <t>house/house015.jpg</t>
-  </si>
-  <si>
-    <t>house/house028.jpg</t>
-  </si>
-  <si>
-    <t>face/face004.jpg</t>
-  </si>
-  <si>
-    <t>house/house017.jpg</t>
-  </si>
-  <si>
-    <t>house/house012.jpg</t>
-  </si>
-  <si>
-    <t>house/house031.jpg</t>
-  </si>
-  <si>
-    <t>face/face027.jpg</t>
-  </si>
-  <si>
-    <t>face/face011.jpg</t>
-  </si>
-  <si>
-    <t>face/face001.jpg</t>
-  </si>
-  <si>
-    <t>house/house009.jpg</t>
-  </si>
-  <si>
-    <t>house/house005.jpg</t>
+    <t>face/face030.jpg</t>
   </si>
   <si>
     <t>house/house007.jpg</t>
   </si>
   <si>
-    <t>face/face026.jpg</t>
-  </si>
-  <si>
-    <t>face/face005.jpg</t>
-  </si>
-  <si>
-    <t>house/house025.jpg</t>
-  </si>
-  <si>
-    <t>face/face003.jpg</t>
-  </si>
-  <si>
-    <t>face/face028.jpg</t>
-  </si>
-  <si>
-    <t>house/house029.jpg</t>
-  </si>
-  <si>
-    <t>face/face029.jpg</t>
-  </si>
-  <si>
-    <t>face/face008.jpg</t>
+    <t>house/house002.jpg</t>
+  </si>
+  <si>
+    <t>face</t>
   </si>
   <si>
     <t>house</t>
-  </si>
-  <si>
-    <t>face</t>
   </si>
 </sst>
 </file>
@@ -709,7 +709,7 @@
         <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -742,7 +742,7 @@
         <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -775,7 +775,7 @@
         <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -830,7 +830,7 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -863,7 +863,7 @@
         <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -874,7 +874,7 @@
         <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -896,7 +896,7 @@
         <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -940,7 +940,7 @@
         <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -962,7 +962,7 @@
         <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1006,7 +1006,7 @@
         <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1105,7 +1105,7 @@
         <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1127,7 +1127,7 @@
         <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:3">

</xml_diff>